<commit_message>
Add evaluation of Teddy dices
</commit_message>
<xml_diff>
--- a/kri-evaluation/results/KRI Liver Segmentation Evaluation v3.xlsx
+++ b/kri-evaluation/results/KRI Liver Segmentation Evaluation v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Master thesis\master\kri-evaluation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAC2D2B-FA2F-4A8B-A960-AE523DD3071E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25093D4-6E0C-460C-827A-64E629B5BCFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2100" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kri" sheetId="1" r:id="rId1"/>
@@ -968,75 +968,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1048,9 +979,6 @@
     </xf>
     <xf numFmtId="1" fontId="7" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1108,6 +1036,78 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5853,9 +5853,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W192"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S47" sqref="S47"/>
+      <selection pane="topRight" activeCell="A75" sqref="A75:L75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5864,19 +5864,19 @@
     <col min="2" max="2" width="9.7109375" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" style="96" customWidth="1"/>
+    <col min="5" max="5" width="5" style="72" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" style="47" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="49" customWidth="1"/>
     <col min="8" max="8" width="10" style="48" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" style="96" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" style="72" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" style="27" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" style="29" customWidth="1"/>
     <col min="12" max="12" width="9.42578125" style="41" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" style="96" customWidth="1"/>
+    <col min="13" max="13" width="4.85546875" style="72" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" style="42" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" style="43" customWidth="1"/>
-    <col min="16" max="16" width="4.5703125" style="98" customWidth="1"/>
-    <col min="17" max="17" width="29.140625" style="82" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="74" customWidth="1"/>
+    <col min="17" max="17" width="29.140625" style="58" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="21"/>
     <col min="19" max="19" width="22" style="33" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" style="33" customWidth="1"/>
@@ -5887,47 +5887,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="22" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="84" t="s">
+      <c r="B1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="85" t="s">
+      <c r="D1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="94"/>
-      <c r="F1" s="86" t="s">
+      <c r="E1" s="70"/>
+      <c r="F1" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="87" t="s">
+      <c r="G1" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="88" t="s">
+      <c r="H1" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="94"/>
-      <c r="J1" s="89" t="s">
+      <c r="I1" s="70"/>
+      <c r="J1" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="84" t="s">
+      <c r="K1" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="90" t="s">
+      <c r="L1" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="94"/>
-      <c r="N1" s="91" t="s">
+      <c r="M1" s="70"/>
+      <c r="N1" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="92" t="s">
+      <c r="O1" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="93" t="s">
+      <c r="P1" s="73"/>
+      <c r="Q1" s="69" t="s">
         <v>35</v>
       </c>
       <c r="S1" s="32"/>
@@ -5950,7 +5950,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E2" s="95"/>
+      <c r="E2" s="71"/>
       <c r="F2" s="45">
         <v>1487.85</v>
       </c>
@@ -5961,9 +5961,9 @@
       <c r="H2" s="50">
         <v>0.89539999999999997</v>
       </c>
-      <c r="I2" s="95"/>
+      <c r="I2" s="71"/>
       <c r="K2" s="36"/>
-      <c r="M2" s="95"/>
+      <c r="M2" s="71"/>
       <c r="N2" s="42">
         <v>1574.15</v>
       </c>
@@ -5989,7 +5989,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E3" s="95"/>
+      <c r="E3" s="71"/>
       <c r="F3" s="47">
         <v>430.29</v>
       </c>
@@ -6026,7 +6026,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E4" s="95"/>
+      <c r="E4" s="71"/>
       <c r="F4" s="47">
         <v>2068.66</v>
       </c>
@@ -6045,17 +6045,17 @@
         <f t="shared" ref="O4:O68" si="0">+ABS((N4-C4)/C4)</f>
         <v>0.33170767004341539</v>
       </c>
-      <c r="Q4" s="82" t="s">
+      <c r="Q4" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="S4" s="61" t="s">
+      <c r="S4" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="T4" s="61"/>
-      <c r="V4" s="64" t="s">
+      <c r="T4" s="89"/>
+      <c r="V4" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="W4" s="65"/>
+      <c r="W4" s="84"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
@@ -6074,7 +6074,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E5" s="95"/>
+      <c r="E5" s="71"/>
       <c r="F5" s="47">
         <v>1813.23</v>
       </c>
@@ -6100,8 +6100,8 @@
         <f>AVERAGEIFS(G2:G104,G2:G104,"&lt;&gt;0",G2:G104,"&lt;30%")</f>
         <v>6.3525422634634648E-2</v>
       </c>
-      <c r="V5" s="66"/>
-      <c r="W5" s="67"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="86"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
@@ -6120,7 +6120,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E6" s="95"/>
+      <c r="E6" s="71"/>
       <c r="F6" s="47">
         <v>1676.44</v>
       </c>
@@ -6146,8 +6146,8 @@
         <f>STDEV(G2:G104)</f>
         <v>0.22863269908852635</v>
       </c>
-      <c r="V6" s="66"/>
-      <c r="W6" s="67"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="86"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="39">
@@ -6166,7 +6166,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E7" s="95"/>
+      <c r="E7" s="71"/>
       <c r="G7" s="46"/>
       <c r="H7" s="51"/>
       <c r="J7" s="27">
@@ -6193,8 +6193,8 @@
         <f>AVERAGEIF(H4:H106,"&lt;&gt;0")</f>
         <v>0.86211363636363636</v>
       </c>
-      <c r="V7" s="66"/>
-      <c r="W7" s="67"/>
+      <c r="V7" s="85"/>
+      <c r="W7" s="86"/>
     </row>
     <row r="8" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="39">
@@ -6213,7 +6213,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E8" s="95"/>
+      <c r="E8" s="71"/>
       <c r="G8" s="46"/>
       <c r="H8" s="51"/>
       <c r="J8" s="27">
@@ -6233,18 +6233,18 @@
         <f t="shared" si="0"/>
         <v>0.33716543730242354</v>
       </c>
-      <c r="Q8" s="82" t="s">
+      <c r="Q8" s="58" t="s">
         <v>42</v>
       </c>
       <c r="S8" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="T8" s="79">
+      <c r="T8" s="56">
         <f>COUNTIF(D2:D104,"=ct")</f>
         <v>46</v>
       </c>
-      <c r="V8" s="68"/>
-      <c r="W8" s="69"/>
+      <c r="V8" s="87"/>
+      <c r="W8" s="88"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
@@ -6263,7 +6263,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E9" s="95"/>
+      <c r="E9" s="71"/>
       <c r="G9" s="46"/>
       <c r="H9" s="51"/>
       <c r="J9" s="27">
@@ -6307,7 +6307,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E10" s="95"/>
+      <c r="E10" s="71"/>
       <c r="F10" s="47">
         <v>1390.57</v>
       </c>
@@ -6350,7 +6350,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E11" s="95"/>
+      <c r="E11" s="71"/>
       <c r="G11" s="46"/>
       <c r="H11" s="51"/>
       <c r="J11" s="27">
@@ -6370,10 +6370,10 @@
         <f t="shared" si="0"/>
         <v>2.6157894736842078E-2</v>
       </c>
-      <c r="V11" s="56" t="s">
+      <c r="V11" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="W11" s="53" t="s">
+      <c r="W11" s="79" t="s">
         <v>54</v>
       </c>
     </row>
@@ -6394,7 +6394,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E12" s="95"/>
+      <c r="E12" s="71"/>
       <c r="G12" s="46"/>
       <c r="H12" s="51"/>
       <c r="J12" s="27">
@@ -6414,12 +6414,12 @@
         <f t="shared" si="0"/>
         <v>9.7069266025434059E-2</v>
       </c>
-      <c r="S12" s="61" t="s">
+      <c r="S12" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="T12" s="61"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="54"/>
+      <c r="T12" s="89"/>
+      <c r="V12" s="77"/>
+      <c r="W12" s="80"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="39">
@@ -6438,7 +6438,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E13" s="95"/>
+      <c r="E13" s="71"/>
       <c r="F13" s="47">
         <v>1374.88</v>
       </c>
@@ -6462,10 +6462,10 @@
       </c>
       <c r="T13" s="34">
         <f>AVERAGEIFS(K2:K104,K2:K104,"&lt;&gt;0",K2:K104,"&lt;30%")</f>
-        <v>5.5947315428946251E-2</v>
-      </c>
-      <c r="V13" s="57"/>
-      <c r="W13" s="54"/>
+        <v>5.1831218923274087E-2</v>
+      </c>
+      <c r="V13" s="77"/>
+      <c r="W13" s="80"/>
     </row>
     <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="39">
@@ -6484,7 +6484,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E14" s="95"/>
+      <c r="E14" s="71"/>
       <c r="G14" s="46"/>
       <c r="H14" s="51"/>
       <c r="J14" s="27">
@@ -6509,10 +6509,10 @@
       </c>
       <c r="T14" s="34">
         <f>STDEV(K2:K104)</f>
-        <v>6.5210044514986645E-2</v>
-      </c>
-      <c r="V14" s="57"/>
-      <c r="W14" s="54"/>
+        <v>6.1011317016409709E-2</v>
+      </c>
+      <c r="V14" s="77"/>
+      <c r="W14" s="80"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="39">
@@ -6531,7 +6531,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E15" s="95"/>
+      <c r="E15" s="71"/>
       <c r="F15" s="47">
         <v>1544.65</v>
       </c>
@@ -6555,10 +6555,10 @@
       </c>
       <c r="T15" s="34">
         <f>AVERAGEIF(L4:L106,"&lt;&gt;0")</f>
-        <v>0.91597428301886796</v>
-      </c>
-      <c r="V15" s="59"/>
-      <c r="W15" s="60"/>
+        <v>0.91841766666666669</v>
+      </c>
+      <c r="V15" s="90"/>
+      <c r="W15" s="91"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="39">
@@ -6577,7 +6577,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E16" s="95"/>
+      <c r="E16" s="71"/>
       <c r="F16" s="47">
         <v>2029.93</v>
       </c>
@@ -6599,14 +6599,14 @@
       <c r="S16" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="T16" s="79">
+      <c r="T16" s="56">
         <f>COUNTIF(D2:D104,"=mr")</f>
         <v>55</v>
       </c>
-      <c r="V16" s="56" t="s">
+      <c r="V16" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="W16" s="53" t="s">
+      <c r="W16" s="79" t="s">
         <v>53</v>
       </c>
     </row>
@@ -6627,7 +6627,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E17" s="95"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="47">
         <v>1818.16</v>
       </c>
@@ -6646,8 +6646,8 @@
         <f t="shared" si="0"/>
         <v>4.5985280283326576E-3</v>
       </c>
-      <c r="V17" s="57"/>
-      <c r="W17" s="54"/>
+      <c r="V17" s="77"/>
+      <c r="W17" s="80"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="39">
@@ -6666,7 +6666,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E18" s="95"/>
+      <c r="E18" s="71"/>
       <c r="F18" s="47">
         <v>360.16</v>
       </c>
@@ -6685,8 +6685,8 @@
         <f t="shared" si="0"/>
         <v>0.12280783272485894</v>
       </c>
-      <c r="V18" s="57"/>
-      <c r="W18" s="54"/>
+      <c r="V18" s="77"/>
+      <c r="W18" s="80"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="39">
@@ -6705,7 +6705,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E19" s="95"/>
+      <c r="E19" s="71"/>
       <c r="F19" s="47">
         <v>2042.57</v>
       </c>
@@ -6724,8 +6724,8 @@
         <f t="shared" si="0"/>
         <v>0.18575885120079233</v>
       </c>
-      <c r="V19" s="57"/>
-      <c r="W19" s="54"/>
+      <c r="V19" s="77"/>
+      <c r="W19" s="80"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="39">
@@ -6744,7 +6744,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E20" s="95"/>
+      <c r="E20" s="71"/>
       <c r="F20" s="47">
         <v>1505.96</v>
       </c>
@@ -6763,12 +6763,12 @@
         <f t="shared" si="0"/>
         <v>0.17690638561686292</v>
       </c>
-      <c r="S20" s="62" t="s">
+      <c r="S20" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="T20" s="63"/>
-      <c r="V20" s="59"/>
-      <c r="W20" s="60"/>
+      <c r="T20" s="99"/>
+      <c r="V20" s="90"/>
+      <c r="W20" s="91"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="39">
@@ -6787,7 +6787,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E21" s="95"/>
+      <c r="E21" s="71"/>
       <c r="G21" s="46"/>
       <c r="H21" s="51"/>
       <c r="J21" s="27">
@@ -6814,10 +6814,10 @@
         <f>AVERAGEIFS(O2:O104,O2:O104,"&lt;&gt;0",O2:O104,"&lt;50%")</f>
         <v>0.13379201009127831</v>
       </c>
-      <c r="V21" s="56" t="s">
+      <c r="V21" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="W21" s="53" t="s">
+      <c r="W21" s="79" t="s">
         <v>30</v>
       </c>
     </row>
@@ -6838,7 +6838,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E22" s="95"/>
+      <c r="E22" s="71"/>
       <c r="G22" s="46"/>
       <c r="H22" s="51"/>
       <c r="J22" s="27">
@@ -6865,8 +6865,8 @@
         <f>STDEV(O2:O104)</f>
         <v>0.16965740518188058</v>
       </c>
-      <c r="V22" s="57"/>
-      <c r="W22" s="54"/>
+      <c r="V22" s="77"/>
+      <c r="W22" s="80"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="39">
@@ -6885,7 +6885,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E23" s="95"/>
+      <c r="E23" s="71"/>
       <c r="G23" s="46"/>
       <c r="H23" s="51"/>
       <c r="J23" s="27">
@@ -6912,8 +6912,8 @@
         <f>STDEV(O3:O105)</f>
         <v>0.17015865056001084</v>
       </c>
-      <c r="V23" s="57"/>
-      <c r="W23" s="54"/>
+      <c r="V23" s="77"/>
+      <c r="W23" s="80"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="39">
@@ -6932,7 +6932,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E24" s="95"/>
+      <c r="E24" s="71"/>
       <c r="G24" s="46"/>
       <c r="H24" s="51"/>
       <c r="J24" s="27">
@@ -6952,9 +6952,9 @@
         <f t="shared" si="0"/>
         <v>0.16852443154329944</v>
       </c>
-      <c r="P24" s="99"/>
-      <c r="V24" s="57"/>
-      <c r="W24" s="54"/>
+      <c r="P24" s="75"/>
+      <c r="V24" s="77"/>
+      <c r="W24" s="80"/>
     </row>
     <row r="25" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="39">
@@ -6973,7 +6973,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E25" s="95"/>
+      <c r="E25" s="71"/>
       <c r="F25" s="47">
         <v>1775.63</v>
       </c>
@@ -6992,8 +6992,8 @@
         <f t="shared" si="0"/>
         <v>0.24993303111477427</v>
       </c>
-      <c r="V25" s="58"/>
-      <c r="W25" s="55"/>
+      <c r="V25" s="78"/>
+      <c r="W25" s="81"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="39">
@@ -7012,7 +7012,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E26" s="95"/>
+      <c r="E26" s="71"/>
       <c r="G26" s="46"/>
       <c r="H26" s="51"/>
       <c r="J26" s="27">
@@ -7032,10 +7032,10 @@
         <f t="shared" si="0"/>
         <v>0.17338942939784374</v>
       </c>
-      <c r="V26" s="70" t="s">
+      <c r="V26" s="92" t="s">
         <v>56</v>
       </c>
-      <c r="W26" s="71"/>
+      <c r="W26" s="93"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="39">
@@ -7054,7 +7054,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E27" s="95"/>
+      <c r="E27" s="71"/>
       <c r="G27" s="46"/>
       <c r="H27" s="51"/>
       <c r="J27" s="27">
@@ -7074,8 +7074,8 @@
         <f t="shared" si="0"/>
         <v>0.13298224292755387</v>
       </c>
-      <c r="V27" s="72"/>
-      <c r="W27" s="73"/>
+      <c r="V27" s="94"/>
+      <c r="W27" s="95"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="39">
@@ -7094,7 +7094,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E28" s="95"/>
+      <c r="E28" s="71"/>
       <c r="F28" s="47">
         <v>1171.33</v>
       </c>
@@ -7113,8 +7113,8 @@
         <f t="shared" si="0"/>
         <v>3.0172777075431905E-2</v>
       </c>
-      <c r="V28" s="72"/>
-      <c r="W28" s="73"/>
+      <c r="V28" s="94"/>
+      <c r="W28" s="95"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="39">
@@ -7133,7 +7133,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E29" s="95"/>
+      <c r="E29" s="71"/>
       <c r="G29" s="46"/>
       <c r="H29" s="51"/>
       <c r="J29" s="27">
@@ -7143,6 +7143,9 @@
         <f t="shared" ref="K29" si="4">+ABS((C29-J29)/C29)</f>
         <v>6.231139816824597E-2</v>
       </c>
+      <c r="L29" s="41">
+        <v>0.93840000000000001</v>
+      </c>
       <c r="N29" s="27">
         <v>1977.03</v>
       </c>
@@ -7150,9 +7153,9 @@
         <f t="shared" si="0"/>
         <v>4.6656784371856573E-2</v>
       </c>
-      <c r="P29" s="99"/>
-      <c r="V29" s="72"/>
-      <c r="W29" s="73"/>
+      <c r="P29" s="75"/>
+      <c r="V29" s="94"/>
+      <c r="W29" s="95"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="39">
@@ -7171,7 +7174,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E30" s="95"/>
+      <c r="E30" s="71"/>
       <c r="F30" s="47">
         <v>1328.99</v>
       </c>
@@ -7190,9 +7193,9 @@
         <f t="shared" si="0"/>
         <v>0.11378577393152652</v>
       </c>
-      <c r="P30" s="99"/>
-      <c r="V30" s="72"/>
-      <c r="W30" s="73"/>
+      <c r="P30" s="75"/>
+      <c r="V30" s="94"/>
+      <c r="W30" s="95"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
@@ -7211,7 +7214,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E31" s="95"/>
+      <c r="E31" s="71"/>
       <c r="G31" s="46"/>
       <c r="H31" s="51"/>
       <c r="J31" s="27">
@@ -7231,8 +7234,8 @@
         <f t="shared" si="0"/>
         <v>0.32840989044125041</v>
       </c>
-      <c r="V31" s="72"/>
-      <c r="W31" s="73"/>
+      <c r="V31" s="94"/>
+      <c r="W31" s="95"/>
     </row>
     <row r="32" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="39">
@@ -7251,7 +7254,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E32" s="95"/>
+      <c r="E32" s="71"/>
       <c r="F32" s="47">
         <v>1607.99</v>
       </c>
@@ -7270,8 +7273,8 @@
         <f t="shared" si="0"/>
         <v>0.12921987692714879</v>
       </c>
-      <c r="V32" s="74"/>
-      <c r="W32" s="75"/>
+      <c r="V32" s="96"/>
+      <c r="W32" s="97"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="39">
@@ -7290,7 +7293,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E33" s="95"/>
+      <c r="E33" s="71"/>
       <c r="F33" s="47">
         <v>1054.97</v>
       </c>
@@ -7327,7 +7330,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E34" s="95"/>
+      <c r="E34" s="71"/>
       <c r="F34" s="47">
         <v>1566.83</v>
       </c>
@@ -7364,7 +7367,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E35" s="95"/>
+      <c r="E35" s="71"/>
       <c r="G35" s="46"/>
       <c r="H35" s="51"/>
       <c r="J35" s="27">
@@ -7384,7 +7387,7 @@
         <f t="shared" si="0"/>
         <v>0.19824656264483229</v>
       </c>
-      <c r="Q35" s="82" t="s">
+      <c r="Q35" s="58" t="s">
         <v>32</v>
       </c>
     </row>
@@ -7405,7 +7408,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E36" s="95"/>
+      <c r="E36" s="71"/>
       <c r="F36" s="47">
         <v>1150.19</v>
       </c>
@@ -7424,7 +7427,7 @@
         <f t="shared" si="0"/>
         <v>0.15338562798665598</v>
       </c>
-      <c r="Q36" s="82" t="s">
+      <c r="Q36" s="58" t="s">
         <v>32</v>
       </c>
     </row>
@@ -7445,7 +7448,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E37" s="95"/>
+      <c r="E37" s="71"/>
       <c r="G37" s="46"/>
       <c r="H37" s="51"/>
       <c r="J37" s="27">
@@ -7465,7 +7468,7 @@
         <f t="shared" si="0"/>
         <v>0.14867331576966503</v>
       </c>
-      <c r="P37" s="99"/>
+      <c r="P37" s="75"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="39">
@@ -7484,7 +7487,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E38" s="95"/>
+      <c r="E38" s="71"/>
       <c r="G38" s="46"/>
       <c r="H38" s="51"/>
       <c r="J38" s="27">
@@ -7522,7 +7525,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E39" s="95"/>
+      <c r="E39" s="71"/>
       <c r="F39" s="47">
         <v>3079.66</v>
       </c>
@@ -7562,7 +7565,7 @@
       <c r="G40" s="46"/>
       <c r="H40" s="51"/>
       <c r="K40" s="36"/>
-      <c r="Q40" s="82" t="s">
+      <c r="Q40" s="58" t="s">
         <v>33</v>
       </c>
     </row>
@@ -7583,7 +7586,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E41" s="95"/>
+      <c r="E41" s="71"/>
       <c r="G41" s="46"/>
       <c r="H41" s="51"/>
       <c r="J41" s="27">
@@ -7621,7 +7624,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E42" s="95"/>
+      <c r="E42" s="71"/>
       <c r="G42" s="46"/>
       <c r="H42" s="51"/>
       <c r="J42" s="27">
@@ -7641,7 +7644,7 @@
         <f t="shared" si="0"/>
         <v>0.22922685129919232</v>
       </c>
-      <c r="P42" s="99"/>
+      <c r="P42" s="75"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="39">
@@ -7660,18 +7663,18 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E43" s="95"/>
+      <c r="E43" s="71"/>
       <c r="G43" s="46"/>
       <c r="H43" s="51"/>
       <c r="J43" s="47">
-        <v>2161.6999999999998</v>
-      </c>
-      <c r="K43" s="76">
+        <v>2860.97</v>
+      </c>
+      <c r="K43" s="53">
         <f t="shared" si="1"/>
-        <v>0.23311338158081465</v>
-      </c>
-      <c r="L43" s="77">
-        <v>0.789883</v>
+        <v>1.4960266780190015E-2</v>
+      </c>
+      <c r="L43" s="54">
+        <v>0.89939999999999998</v>
       </c>
       <c r="N43" s="42">
         <v>3256.97</v>
@@ -7698,7 +7701,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E44" s="95"/>
+      <c r="E44" s="71"/>
       <c r="F44" s="47">
         <v>2911.33</v>
       </c>
@@ -7717,7 +7720,7 @@
         <f t="shared" si="0"/>
         <v>0.21943104582328443</v>
       </c>
-      <c r="Q44" s="82" t="s">
+      <c r="Q44" s="58" t="s">
         <v>31</v>
       </c>
     </row>
@@ -7738,7 +7741,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E45" s="95"/>
+      <c r="E45" s="71"/>
       <c r="G45" s="46"/>
       <c r="H45" s="51"/>
       <c r="K45" s="36"/>
@@ -7749,7 +7752,7 @@
         <f t="shared" si="0"/>
         <v>9.7401334688646465E-2</v>
       </c>
-      <c r="Q45" s="82" t="s">
+      <c r="Q45" s="58" t="s">
         <v>55</v>
       </c>
     </row>
@@ -7770,7 +7773,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E46" s="95"/>
+      <c r="E46" s="71"/>
       <c r="F46" s="47">
         <v>1306.32</v>
       </c>
@@ -7807,7 +7810,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E47" s="95"/>
+      <c r="E47" s="71"/>
       <c r="G47" s="46"/>
       <c r="H47" s="51"/>
       <c r="J47" s="27">
@@ -7845,7 +7848,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E48" s="95"/>
+      <c r="E48" s="71"/>
       <c r="F48" s="47">
         <v>1284.98</v>
       </c>
@@ -7882,7 +7885,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E49" s="95"/>
+      <c r="E49" s="71"/>
       <c r="F49" s="47">
         <v>1320.03</v>
       </c>
@@ -7919,7 +7922,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E50" s="95"/>
+      <c r="E50" s="71"/>
       <c r="G50" s="46"/>
       <c r="H50" s="51"/>
       <c r="J50" s="27">
@@ -7957,7 +7960,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E51" s="95"/>
+      <c r="E51" s="71"/>
       <c r="G51" s="46"/>
       <c r="H51" s="51"/>
       <c r="J51" s="27">
@@ -7995,7 +7998,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E52" s="95"/>
+      <c r="E52" s="71"/>
       <c r="F52" s="47">
         <v>204.72800000000001</v>
       </c>
@@ -8032,7 +8035,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E53" s="95"/>
+      <c r="E53" s="71"/>
       <c r="F53" s="47">
         <v>2132.17</v>
       </c>
@@ -8069,7 +8072,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E54" s="95"/>
+      <c r="E54" s="71"/>
       <c r="F54" s="47">
         <v>3118.28</v>
       </c>
@@ -8106,7 +8109,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E55" s="95"/>
+      <c r="E55" s="71"/>
       <c r="F55" s="47">
         <v>1897.91</v>
       </c>
@@ -8143,7 +8146,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E56" s="95"/>
+      <c r="E56" s="71"/>
       <c r="G56" s="46"/>
       <c r="H56" s="51"/>
       <c r="J56" s="27">
@@ -8181,7 +8184,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E57" s="95"/>
+      <c r="E57" s="71"/>
       <c r="G57" s="46"/>
       <c r="H57" s="51"/>
       <c r="J57" s="27">
@@ -8219,7 +8222,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E58" s="95"/>
+      <c r="E58" s="71"/>
       <c r="F58" s="47">
         <v>1604.75</v>
       </c>
@@ -8256,7 +8259,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E59" s="95"/>
+      <c r="E59" s="71"/>
       <c r="F59" s="47">
         <v>1791.65</v>
       </c>
@@ -8293,7 +8296,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E60" s="95"/>
+      <c r="E60" s="71"/>
       <c r="F60" s="47">
         <v>1426.29</v>
       </c>
@@ -8330,7 +8333,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E61" s="95"/>
+      <c r="E61" s="71"/>
       <c r="F61" s="47">
         <v>1965.81</v>
       </c>
@@ -8367,7 +8370,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E62" s="95"/>
+      <c r="E62" s="71"/>
       <c r="F62" s="47">
         <v>1285.73</v>
       </c>
@@ -8404,7 +8407,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E63" s="95"/>
+      <c r="E63" s="71"/>
       <c r="G63" s="46"/>
       <c r="H63" s="51"/>
       <c r="J63" s="27">
@@ -8442,7 +8445,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E64" s="95"/>
+      <c r="E64" s="71"/>
       <c r="F64" s="47">
         <v>1369.12</v>
       </c>
@@ -8479,7 +8482,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E65" s="95"/>
+      <c r="E65" s="71"/>
       <c r="F65" s="47">
         <v>1197.28</v>
       </c>
@@ -8516,7 +8519,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E66" s="95"/>
+      <c r="E66" s="71"/>
       <c r="F66" s="47">
         <v>1388.7</v>
       </c>
@@ -8535,7 +8538,7 @@
         <f t="shared" si="0"/>
         <v>0.30868192580899756</v>
       </c>
-      <c r="Q66" s="82" t="s">
+      <c r="Q66" s="58" t="s">
         <v>39</v>
       </c>
     </row>
@@ -8556,7 +8559,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E67" s="95"/>
+      <c r="E67" s="71"/>
       <c r="G67" s="46"/>
       <c r="H67" s="51"/>
       <c r="J67" s="27">
@@ -8594,7 +8597,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E68" s="95"/>
+      <c r="E68" s="71"/>
       <c r="G68" s="46"/>
       <c r="H68" s="51"/>
       <c r="J68" s="27">
@@ -8632,7 +8635,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E69" s="95"/>
+      <c r="E69" s="71"/>
       <c r="F69" s="47">
         <v>2330.11</v>
       </c>
@@ -8669,7 +8672,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E70" s="95"/>
+      <c r="E70" s="71"/>
       <c r="G70" s="46"/>
       <c r="H70" s="51"/>
       <c r="J70" s="27">
@@ -8707,7 +8710,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E71" s="95"/>
+      <c r="E71" s="71"/>
       <c r="G71" s="46"/>
       <c r="H71" s="51"/>
       <c r="J71" s="27">
@@ -8745,17 +8748,17 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E72" s="95"/>
+      <c r="E72" s="71"/>
       <c r="G72" s="46"/>
       <c r="H72" s="51"/>
       <c r="J72" s="47">
         <v>2166.4899999999998</v>
       </c>
-      <c r="K72" s="76">
+      <c r="K72" s="53">
         <f t="shared" si="5"/>
         <v>0.20370125335391631</v>
       </c>
-      <c r="L72" s="77">
+      <c r="L72" s="54">
         <v>0.90966199999999997</v>
       </c>
       <c r="N72" s="42">
@@ -8783,7 +8786,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E73" s="95"/>
+      <c r="E73" s="71"/>
       <c r="F73" s="47">
         <v>1878.56</v>
       </c>
@@ -8802,7 +8805,7 @@
         <f t="shared" si="6"/>
         <v>0.29715020576131679</v>
       </c>
-      <c r="Q73" s="82" t="s">
+      <c r="Q73" s="58" t="s">
         <v>39</v>
       </c>
     </row>
@@ -8823,7 +8826,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E74" s="95"/>
+      <c r="E74" s="71"/>
       <c r="F74" s="47">
         <v>1489.32</v>
       </c>
@@ -8842,7 +8845,7 @@
         <f t="shared" si="6"/>
         <v>0.13200887323024724</v>
       </c>
-      <c r="P74" s="99"/>
+      <c r="P74" s="75"/>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="39">
@@ -8861,7 +8864,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E75" s="95"/>
+      <c r="E75" s="71"/>
       <c r="G75" s="46"/>
       <c r="H75" s="51"/>
       <c r="J75" s="27">
@@ -8899,7 +8902,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E76" s="95"/>
+      <c r="E76" s="71"/>
       <c r="G76" s="46"/>
       <c r="H76" s="51"/>
       <c r="J76" s="27">
@@ -8937,7 +8940,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E77" s="95"/>
+      <c r="E77" s="71"/>
       <c r="F77" s="47">
         <v>1673.78</v>
       </c>
@@ -8974,7 +8977,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E78" s="95"/>
+      <c r="E78" s="71"/>
       <c r="F78" s="47">
         <v>1796.36</v>
       </c>
@@ -9011,7 +9014,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E79" s="95"/>
+      <c r="E79" s="71"/>
       <c r="G79" s="46"/>
       <c r="H79" s="51"/>
       <c r="J79" s="27">
@@ -9049,7 +9052,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E80" s="95"/>
+      <c r="E80" s="71"/>
       <c r="G80" s="46"/>
       <c r="H80" s="51"/>
       <c r="J80" s="27">
@@ -9087,7 +9090,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E81" s="95"/>
+      <c r="E81" s="71"/>
       <c r="G81" s="46"/>
       <c r="H81" s="51"/>
       <c r="J81" s="27">
@@ -9125,7 +9128,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E82" s="95"/>
+      <c r="E82" s="71"/>
       <c r="G82" s="46"/>
       <c r="H82" s="51"/>
       <c r="J82" s="27">
@@ -9163,7 +9166,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E83" s="95"/>
+      <c r="E83" s="71"/>
       <c r="G83" s="46"/>
       <c r="H83" s="51"/>
       <c r="J83" s="27">
@@ -9201,7 +9204,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E84" s="95"/>
+      <c r="E84" s="71"/>
       <c r="G84" s="46"/>
       <c r="H84" s="51"/>
       <c r="J84" s="27">
@@ -9239,7 +9242,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E85" s="95"/>
+      <c r="E85" s="71"/>
       <c r="F85" s="47">
         <v>1902.79</v>
       </c>
@@ -9275,7 +9278,7 @@
       <c r="D86" s="40">
         <v>0</v>
       </c>
-      <c r="E86" s="95"/>
+      <c r="E86" s="71"/>
       <c r="G86" s="46"/>
       <c r="H86" s="51"/>
       <c r="K86" s="36"/>
@@ -9297,7 +9300,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E87" s="95"/>
+      <c r="E87" s="71"/>
       <c r="G87" s="46"/>
       <c r="H87" s="51"/>
       <c r="J87" s="27">
@@ -9335,7 +9338,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E88" s="95"/>
+      <c r="E88" s="71"/>
       <c r="F88" s="47">
         <v>864.98</v>
       </c>
@@ -9372,7 +9375,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E89" s="95"/>
+      <c r="E89" s="71"/>
       <c r="G89" s="46"/>
       <c r="H89" s="51"/>
       <c r="J89" s="27">
@@ -9410,7 +9413,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E90" s="95"/>
+      <c r="E90" s="71"/>
       <c r="F90" s="47">
         <v>1043.18</v>
       </c>
@@ -9429,7 +9432,7 @@
         <f t="shared" si="8"/>
         <v>0.85086058952357013</v>
       </c>
-      <c r="Q90" s="82" t="s">
+      <c r="Q90" s="58" t="s">
         <v>42</v>
       </c>
     </row>
@@ -9450,7 +9453,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E91" s="95"/>
+      <c r="E91" s="71"/>
       <c r="G91" s="46"/>
       <c r="H91" s="51"/>
       <c r="J91" s="27">
@@ -9488,7 +9491,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E92" s="95"/>
+      <c r="E92" s="71"/>
       <c r="G92" s="46"/>
       <c r="H92" s="51"/>
       <c r="J92" s="27">
@@ -9526,7 +9529,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E93" s="95"/>
+      <c r="E93" s="71"/>
       <c r="G93" s="46"/>
       <c r="H93" s="51"/>
       <c r="J93" s="27">
@@ -9564,7 +9567,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E94" s="95"/>
+      <c r="E94" s="71"/>
       <c r="G94" s="46"/>
       <c r="H94" s="51"/>
       <c r="J94" s="27">
@@ -9602,7 +9605,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E95" s="95"/>
+      <c r="E95" s="71"/>
       <c r="G95" s="46"/>
       <c r="H95" s="51"/>
       <c r="J95" s="27">
@@ -9640,7 +9643,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E96" s="95"/>
+      <c r="E96" s="71"/>
       <c r="G96" s="46"/>
       <c r="H96" s="51"/>
       <c r="J96" s="27">
@@ -9678,7 +9681,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E97" s="95"/>
+      <c r="E97" s="71"/>
       <c r="G97" s="46"/>
       <c r="H97" s="51"/>
       <c r="J97" s="27">
@@ -9716,7 +9719,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E98" s="95"/>
+      <c r="E98" s="71"/>
       <c r="G98" s="46"/>
       <c r="H98" s="51"/>
       <c r="J98" s="27">
@@ -9754,7 +9757,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E99" s="95"/>
+      <c r="E99" s="71"/>
       <c r="G99" s="46"/>
       <c r="H99" s="51"/>
       <c r="J99" s="27">
@@ -9792,7 +9795,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E100" s="95"/>
+      <c r="E100" s="71"/>
       <c r="G100" s="46"/>
       <c r="H100" s="51"/>
       <c r="J100" s="27">
@@ -9830,7 +9833,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E101" s="95"/>
+      <c r="E101" s="71"/>
       <c r="G101" s="46"/>
       <c r="H101" s="51"/>
       <c r="J101" s="27">
@@ -9868,7 +9871,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>ct</v>
       </c>
-      <c r="E102" s="95"/>
+      <c r="E102" s="71"/>
       <c r="F102" s="47">
         <v>3521.54</v>
       </c>
@@ -9887,7 +9890,7 @@
         <f t="shared" si="8"/>
         <v>0.12450133159410846</v>
       </c>
-      <c r="Q102" s="82" t="s">
+      <c r="Q102" s="58" t="s">
         <v>39</v>
       </c>
     </row>
@@ -9908,16 +9911,16 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E103" s="95"/>
+      <c r="E103" s="71"/>
       <c r="G103" s="46"/>
       <c r="J103" s="47">
         <v>1988.8</v>
       </c>
-      <c r="K103" s="78">
+      <c r="K103" s="55">
         <f t="shared" si="5"/>
         <v>0.36546515619636111</v>
       </c>
-      <c r="L103" s="77">
+      <c r="L103" s="54">
         <v>0.80160799999999999</v>
       </c>
       <c r="N103" s="42">
@@ -9927,7 +9930,7 @@
         <f t="shared" si="8"/>
         <v>0.73837555784414688</v>
       </c>
-      <c r="Q103" s="82" t="s">
+      <c r="Q103" s="58" t="s">
         <v>42</v>
       </c>
     </row>
@@ -9948,7 +9951,7 @@
         <f>+Table1[[#This Row],[Modality]]</f>
         <v>mr</v>
       </c>
-      <c r="E104" s="95"/>
+      <c r="E104" s="71"/>
       <c r="G104" s="46"/>
       <c r="J104" s="27">
         <v>1781.79</v>
@@ -9975,15 +9978,15 @@
       <c r="K106" s="37"/>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B107" s="80"/>
-      <c r="C107" s="80"/>
-      <c r="D107" s="81"/>
+      <c r="B107" s="82"/>
+      <c r="C107" s="82"/>
+      <c r="D107" s="57"/>
       <c r="K107" s="37"/>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B108" s="80"/>
-      <c r="C108" s="80"/>
-      <c r="D108" s="81"/>
+      <c r="B108" s="82"/>
+      <c r="C108" s="82"/>
+      <c r="D108" s="57"/>
       <c r="K108" s="37"/>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
@@ -10319,7 +10322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -10331,6 +10334,22 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DLCPolicyLabelClientValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">{_UIVersionString}</DLCPolicyLabelClientValue>
+    <_dlc_BarcodeImage xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">iVBORw0KGgoAAAANSUhEUgAAAYIAAABtCAYAAACsn2ZqAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAADsMAAA7DAcdvqGQAABp9SURBVHhe7ZvBihzbsiz3///0eeiBgeGE54qsTA0uSgMfWLt3aA2aqpH++9/Hx8fHxz/N90Xw8fHx8Y/zfRF8fHx8/ON8XwQfHx8f/zjfF8HHx8fHP873RfDx8fHxj/P6F8F///33/zORHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef/ix8fHx8f/Kb4vgo+Pj49/nO+L4OPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+/irtP7/wH2OmwNQRc9XBWxu46k93snfMVffx8SbfX9fHX+XuB5j3m9+dNvmztzamdb/+W8nmzsfHW3x/WR9/hT8fWmRLbk+/e9XTbTZX5OaPk+Tqnrur3Yknv/vx0fj+qj7+Knc+uHJ7+t2rnm6zuaJtpp9v/63Nv9t48rsfH43vr+rjr7L94Jp2f36WSU4/m3q46v7wy+9OP8+f/fHMljvbj48t31/Vx19l+8H1ZPfnZ46Z9jB17U5yuru9A5vd9tbHx12+v6yPv8rf+IDzfvrd/FnbTD83V33r2r+14Zd/7+PjDb6/ro+/yuYD7O6HHPs7H5x/3OFnJ9pm+vnVvbf/rY+PN/n+wj7+KqcPsV8+5Pidq9/d3H2ymX7+N96z+b2Pj6d8f2Uff5XTB9kvH3T8ztXvvvXvtt308yfv+UNuNr/z8fEG31/ax1/lyYfj1G8+LN+4+4erO63b3Pl18/Hxt/j+2j7+Cn8+yDLJ9LPkdOMPp82ph80uN9Pu1P/htMne+fh4m++v6uPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+Pj4+/nG+L4KPj4+Pf5r//e//AYQWEYJwHQKsAAAAAElFTkSuQmCC</_dlc_BarcodeImage>
+    <DLCPolicyLabelLock xmlns="e2656bbd-0e15-4aa0-af00-25744e385561" xsi:nil="true"/>
+    <_dlc_BarcodeValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">1758931852</_dlc_BarcodeValue>
+    <_dlc_BarcodePreview xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">
+      <Url>https://surgiceye.sharepoint.com/dev/_layouts/15/barcodeimagefromitem.aspx?ID=419111&amp;list=e2656bbd-0e15-4aa0-af00-25744e385561</Url>
+      <Description>Barcode: 1758931852</Description>
+    </_dlc_BarcodePreview>
+    <DLCPolicyLabelValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">0.3</DLCPolicyLabelValue>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="SurgicEye WordTemplate" ma:contentTypeID="0x01010074A3F29CB79E8A41A92E73E19AE321CB00098C261D3F46DB49AEA371869FEC377C" ma:contentTypeVersion="17" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="d27efd9bfa2cf0dc081f61d6777772ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e2656bbd-0e15-4aa0-af00-25744e385561" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53fececc5845ce19907e3af2573e5d2e" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10506,32 +10525,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DLCPolicyLabelClientValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">{_UIVersionString}</DLCPolicyLabelClientValue>
-    <_dlc_BarcodeImage xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">iVBORw0KGgoAAAANSUhEUgAAAYIAAABtCAYAAACsn2ZqAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAADsMAAA7DAcdvqGQAABp9SURBVHhe7ZvBihzbsiz3///0eeiBgeGE54qsTA0uSgMfWLt3aA2aqpH++9/Hx8fHxz/N90Xw8fHx8Y/zfRF8fHx8/ON8XwQfHx8f/zjfF8HHx8fHP873RfDx8fHxj/P6F8F///33/zORHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef/ix8fHx8f/Kb4vgo+Pj49/nO+L4OPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+/irtP7/wH2OmwNQRc9XBWxu46k93snfMVffx8SbfX9fHX+XuB5j3m9+dNvmztzamdb/+W8nmzsfHW3x/WR9/hT8fWmRLbk+/e9XTbTZX5OaPk+Tqnrur3Yknv/vx0fj+qj7+Knc+uHJ7+t2rnm6zuaJtpp9v/63Nv9t48rsfH43vr+rjr7L94Jp2f36WSU4/m3q46v7wy+9OP8+f/fHMljvbj48t31/Vx19l+8H1ZPfnZ46Z9jB17U5yuru9A5vd9tbHx12+v6yPv8rf+IDzfvrd/FnbTD83V33r2r+14Zd/7+PjDb6/ro+/yuYD7O6HHPs7H5x/3OFnJ9pm+vnVvbf/rY+PN/n+wj7+KqcPsV8+5Pidq9/d3H2ymX7+N96z+b2Pj6d8f2Uff5XTB9kvH3T8ztXvvvXvtt308yfv+UNuNr/z8fEG31/ax1/lyYfj1G8+LN+4+4erO63b3Pl18/Hxt/j+2j7+Cn8+yDLJ9LPkdOMPp82ph80uN9Pu1P/htMne+fh4m++v6uPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+Pj4+/nG+L4KPj4+Pf5r//e//AYQWEYJwHQKsAAAAAElFTkSuQmCC</_dlc_BarcodeImage>
-    <DLCPolicyLabelLock xmlns="e2656bbd-0e15-4aa0-af00-25744e385561" xsi:nil="true"/>
-    <_dlc_BarcodeValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">1758931852</_dlc_BarcodeValue>
-    <_dlc_BarcodePreview xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">
-      <Url>https://surgiceye.sharepoint.com/dev/_layouts/15/barcodeimagefromitem.aspx?ID=419111&amp;list=e2656bbd-0e15-4aa0-af00-25744e385561</Url>
-      <Description>Barcode: 1758931852</Description>
-    </_dlc_BarcodePreview>
-    <DLCPolicyLabelValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">0.3</DLCPolicyLabelValue>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <p:Policy xmlns:p="office.server.policy" id="" local="true">
   <p:Name>SurgicEye WordTemplate</p:Name>
@@ -10558,7 +10552,33 @@
 </p:Policy>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB86876-AAC8-4339-8E74-E0DFE2CA9AC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e2656bbd-0e15-4aa0-af00-25744e385561"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8953B42-7F0B-4652-8904-3F0A580F556B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10577,35 +10597,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB86876-AAC8-4339-8E74-E0DFE2CA9AC3}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A933A0-2E29-4D82-A4A8-6FECA8CC0598}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="e2656bbd-0e15-4aa0-af00-25744e385561"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="office.server.policy"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3611D48C-6B4F-4CD9-8579-A2A41CE94ADA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A933A0-2E29-4D82-A4A8-6FECA8CC0598}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="office.server.policy"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>